<commit_message>
fetching summary from component
</commit_message>
<xml_diff>
--- a/comp_cname.xlsx
+++ b/comp_cname.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gunjanpanda/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gunjanpanda/Desktop/compIssueCreation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD694B55-FA71-4648-BC8B-F265620398B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B15E76-0087-654E-B0F3-435B1B0170FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20240" xr2:uid="{180643DD-8EE4-E94A-8913-E73A9372F684}"/>
   </bookViews>
@@ -36,72 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Components</t>
   </si>
   <si>
-    <t>Customer_name</t>
-  </si>
-  <si>
     <t>00002 - CSG</t>
   </si>
   <si>
-    <t> CSG</t>
-  </si>
-  <si>
     <t>00007 - LNR Property</t>
   </si>
   <si>
-    <t> LNR Property</t>
-  </si>
-  <si>
     <t>00019 - Performant</t>
   </si>
   <si>
-    <t> Performant</t>
-  </si>
-  <si>
     <t>00039 - Toyo Tire</t>
   </si>
   <si>
-    <t> Toyo Tire</t>
-  </si>
-  <si>
     <t>00040 - Okinawa Institute of Science and Technology</t>
   </si>
   <si>
-    <t> Okinawa Institute of Science and Technology</t>
-  </si>
-  <si>
     <t>00042 - IBM India</t>
   </si>
   <si>
-    <t> IBM India</t>
-  </si>
-  <si>
     <t>00043 - Cognizant - Healogics</t>
   </si>
   <si>
-    <t> Cognizant - Healogics</t>
-  </si>
-  <si>
     <t>00044 - NANA</t>
   </si>
   <si>
-    <t> NANA</t>
-  </si>
-  <si>
     <t>00046 - Capital Markets</t>
   </si>
   <si>
-    <t> Capital Markets</t>
-  </si>
-  <si>
     <t>00052 - MSS - Saputo</t>
-  </si>
-  <si>
-    <t> MSS - Saputo</t>
   </si>
 </sst>
 </file>
@@ -465,7 +432,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,88 +445,56 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>